<commit_message>
updated: docs - Se actualizo la estructura de docs - Se removieron archivos innecesarios - Renombrados algunos archivos
</commit_message>
<xml_diff>
--- a/docs/Historia de usuarios actualizada 24092021.xlsx
+++ b/docs/Historia de usuarios actualizada 24092021.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Datos\ROBERTO\PROYECTOS\mintic-syseducativo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6179AF74-AA19-4B6B-9BB2-6FB8EA9E80B6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{372ADC50-DEE0-4465-BC78-23AEC80BAC55}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Historias de Usuario" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="116">
   <si>
     <t>ID. de la historia</t>
   </si>
@@ -358,13 +357,28 @@
   </si>
   <si>
     <t>ID28</t>
+  </si>
+  <si>
+    <t>Valor</t>
+  </si>
+  <si>
+    <t>Dependencia</t>
+  </si>
+  <si>
+    <t>Sprint</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>Puntuación</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -381,7 +395,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -408,7 +431,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -416,48 +439,59 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -771,11 +805,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{651A1867-1870-4254-AFF7-E2D96FB81DCA}">
-  <dimension ref="A1:H82"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A71" sqref="A71"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,884 +818,759 @@
     <col min="3" max="3" width="31" customWidth="1"/>
     <col min="4" max="4" width="27.7109375" customWidth="1"/>
     <col min="5" max="5" width="34.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-    </row>
-    <row r="2" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+    </row>
+    <row r="2" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="8" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="F2" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="10"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-    </row>
-    <row r="5" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="E3" s="2"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+    </row>
+    <row r="4" spans="1:10" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="10"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="9"/>
-    </row>
-    <row r="7" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="E4" s="2"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+    </row>
+    <row r="5" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="11"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="9"/>
-    </row>
-    <row r="9" spans="1:8" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="E5" s="2"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" spans="1:10" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="11"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="9"/>
-    </row>
-    <row r="11" spans="1:8" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="E6" s="2"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+    </row>
+    <row r="7" spans="1:10" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="11"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="9"/>
-    </row>
-    <row r="13" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="E7" s="2"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+    </row>
+    <row r="8" spans="1:10" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="10"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-    </row>
-    <row r="15" spans="1:8" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="E8" s="2"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" spans="1:10" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="10"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-    </row>
-    <row r="17" spans="1:5" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+      <c r="E9" s="2"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+    </row>
+    <row r="10" spans="1:10" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="10"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-    </row>
-    <row r="19" spans="1:5" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+      <c r="E10" s="2"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+    </row>
+    <row r="11" spans="1:10" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C11" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D11" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E19" s="10"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-    </row>
-    <row r="21" spans="1:5" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
+      <c r="E11" s="2"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+    </row>
+    <row r="12" spans="1:10" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D12" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E21" s="10"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-    </row>
-    <row r="23" spans="1:5" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
+      <c r="E12" s="2"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="1:10" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D13" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E23" s="10"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-    </row>
-    <row r="25" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
+      <c r="E13" s="2"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+    </row>
+    <row r="14" spans="1:10" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D14" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E25" s="10"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-    </row>
-    <row r="27" spans="1:5" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
+      <c r="E14" s="2"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+    </row>
+    <row r="15" spans="1:10" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D15" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E27" s="10"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-    </row>
-    <row r="29" spans="1:5" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
+      <c r="E15" s="2"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+    </row>
+    <row r="16" spans="1:10" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B16" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C16" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D16" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E29" s="10"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-    </row>
-    <row r="31" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="7" t="s">
+      <c r="E16" s="2"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+    </row>
+    <row r="17" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B17" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C17" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="D17" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E31" s="10"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-    </row>
-    <row r="33" spans="1:7" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
+      <c r="E17" s="2"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+    </row>
+    <row r="18" spans="1:10" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B18" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C18" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="D18" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E33" s="10"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-    </row>
-    <row r="35" spans="1:7" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
+      <c r="E18" s="2"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+    </row>
+    <row r="19" spans="1:10" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B19" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="C19" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D35" s="10" t="s">
+      <c r="D19" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E35" s="10"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
-    </row>
-    <row r="37" spans="1:7" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="7" t="s">
+      <c r="E19" s="2"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+    </row>
+    <row r="20" spans="1:10" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B20" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C20" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D37" s="10" t="s">
+      <c r="D20" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E37" s="10"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-    </row>
-    <row r="39" spans="1:7" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="7" t="s">
+      <c r="E20" s="2"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+    </row>
+    <row r="21" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B21" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C39" s="10" t="s">
+      <c r="C21" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D39" s="10" t="s">
+      <c r="D21" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E39" s="10"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-    </row>
-    <row r="41" spans="1:7" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="7" t="s">
+      <c r="E21" s="2"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+    </row>
+    <row r="22" spans="1:10" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B22" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C41" s="10" t="s">
+      <c r="C22" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D41" s="10" t="s">
+      <c r="D22" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E41" s="10"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="6"/>
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-    </row>
-    <row r="43" spans="1:7" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="7" t="s">
+      <c r="E22" s="2"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+    </row>
+    <row r="23" spans="1:10" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B23" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C43" s="10" t="s">
+      <c r="C23" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D43" s="10" t="s">
+      <c r="D23" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E43" s="10"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="6"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
-    </row>
-    <row r="45" spans="1:7" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="7" t="s">
+      <c r="E23" s="2"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+    </row>
+    <row r="24" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="B24" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C45" s="10" t="s">
+      <c r="C24" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D45" s="10" t="s">
+      <c r="D24" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E45" s="10"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="6"/>
-      <c r="B46" s="6"/>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
-    </row>
-    <row r="47" spans="1:7" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="7" t="s">
+      <c r="E24" s="2"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+    </row>
+    <row r="25" spans="1:10" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B47" s="7" t="s">
+      <c r="B25" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C47" s="10" t="s">
+      <c r="C25" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D47" s="10" t="s">
+      <c r="D25" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E47" s="10"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="6"/>
-      <c r="B48" s="6"/>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
-    </row>
-    <row r="49" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="7" t="s">
+      <c r="E25" s="2"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+    </row>
+    <row r="26" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B49" s="7" t="s">
+      <c r="B26" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C49" s="10" t="s">
+      <c r="C26" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D49" s="10" t="s">
+      <c r="D26" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E49" s="10"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="6"/>
-      <c r="B50" s="6"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
-    </row>
-    <row r="51" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="7" t="s">
+      <c r="E26" s="2"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+    </row>
+    <row r="27" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B51" s="7" t="s">
+      <c r="B27" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C51" s="10" t="s">
+      <c r="C27" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D51" s="10" t="s">
+      <c r="D27" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E51" s="10"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="6"/>
-      <c r="B52" s="6"/>
-      <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="6"/>
-    </row>
-    <row r="53" spans="1:5" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="7" t="s">
+      <c r="E27" s="2"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+    </row>
+    <row r="28" spans="1:10" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B53" s="7" t="s">
+      <c r="B28" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C53" s="10" t="s">
+      <c r="C28" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D53" s="10" t="s">
+      <c r="D28" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="E53" s="10"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="6"/>
-      <c r="B54" s="6"/>
-      <c r="C54" s="6"/>
-      <c r="D54" s="6"/>
-      <c r="E54" s="6"/>
-    </row>
-    <row r="55" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="7" t="s">
+      <c r="E28" s="2"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+    </row>
+    <row r="29" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B55" s="7" t="s">
+      <c r="B29" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C55" s="10" t="s">
+      <c r="C29" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D55" s="10" t="s">
+      <c r="D29" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="E55" s="10"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="6"/>
-      <c r="B56" s="6"/>
-      <c r="C56" s="6"/>
-      <c r="D56" s="6"/>
-      <c r="E56" s="6"/>
-    </row>
-    <row r="57" spans="1:5" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="7" t="s">
+      <c r="E29" s="2"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+    </row>
+    <row r="30" spans="1:10" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="B30" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C57" s="10" t="s">
+      <c r="C30" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D57" s="10" t="s">
+      <c r="D30" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="E57" s="10"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="6"/>
-      <c r="B58" s="6"/>
-      <c r="C58" s="6"/>
-      <c r="D58" s="6"/>
-      <c r="E58" s="6"/>
-    </row>
-    <row r="59" spans="1:5" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="7" t="s">
+      <c r="E30" s="2"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+    </row>
+    <row r="31" spans="1:10" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B59" s="7" t="s">
+      <c r="B31" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C59" s="10" t="s">
+      <c r="C31" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D59" s="10" t="s">
+      <c r="D31" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="E59" s="10"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="6"/>
-      <c r="B60" s="6"/>
-      <c r="C60" s="6"/>
-      <c r="D60" s="6"/>
-      <c r="E60" s="6"/>
-    </row>
-    <row r="61" spans="1:5" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="7" t="s">
+      <c r="E31" s="2"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+    </row>
+    <row r="32" spans="1:10" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B61" s="7" t="s">
+      <c r="B32" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C61" s="10" t="s">
+      <c r="C32" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D61" s="10" t="s">
+      <c r="D32" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E61" s="10"/>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="6"/>
-      <c r="B62" s="6"/>
-      <c r="C62" s="6"/>
-      <c r="D62" s="6"/>
-      <c r="E62" s="6"/>
-    </row>
-    <row r="63" spans="1:5" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="7" t="s">
+      <c r="E32" s="2"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+    </row>
+    <row r="33" spans="1:10" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B63" s="7" t="s">
+      <c r="B33" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C63" s="10" t="s">
+      <c r="C33" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D63" s="10" t="s">
+      <c r="D33" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="E63" s="10"/>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="6"/>
-      <c r="B64" s="6"/>
-      <c r="C64" s="6"/>
-      <c r="D64" s="6"/>
-      <c r="E64" s="6"/>
-    </row>
-    <row r="65" spans="1:5" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="7" t="s">
+      <c r="E33" s="2"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
+    </row>
+    <row r="34" spans="1:10" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B65" s="7" t="s">
+      <c r="B34" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C65" s="10" t="s">
+      <c r="C34" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D65" s="10" t="s">
+      <c r="D34" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E65" s="10"/>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="6"/>
-      <c r="B66" s="6"/>
-      <c r="C66" s="6"/>
-      <c r="D66" s="6"/>
-      <c r="E66" s="6"/>
-    </row>
-    <row r="67" spans="1:5" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="7" t="s">
+      <c r="E34" s="2"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+    </row>
+    <row r="35" spans="1:10" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B67" s="7" t="s">
+      <c r="B35" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C67" s="10" t="s">
+      <c r="C35" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D67" s="10" t="s">
+      <c r="D35" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E67" s="10"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="6"/>
-      <c r="B68" s="6"/>
-      <c r="C68" s="6"/>
-      <c r="D68" s="6"/>
-      <c r="E68" s="6"/>
-    </row>
-    <row r="69" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="7" t="s">
+      <c r="E35" s="2"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+    </row>
+    <row r="36" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B69" s="7" t="s">
+      <c r="B36" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C69" s="10" t="s">
+      <c r="C36" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D69" s="10" t="s">
+      <c r="D36" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E69" s="10"/>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="6"/>
-      <c r="B70" s="6"/>
-      <c r="C70" s="6"/>
-      <c r="D70" s="6"/>
-      <c r="E70" s="6"/>
-    </row>
-    <row r="71" spans="1:5" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="7" t="s">
+      <c r="E36" s="2"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
+    </row>
+    <row r="37" spans="1:10" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B71" s="7" t="s">
+      <c r="B37" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C71" s="10" t="s">
+      <c r="C37" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D71" s="10" t="s">
+      <c r="D37" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E71" s="10"/>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="6"/>
-      <c r="B72" s="6"/>
-      <c r="C72" s="6"/>
-      <c r="D72" s="6"/>
-      <c r="E72" s="6"/>
-    </row>
-    <row r="73" spans="1:5" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="7"/>
-      <c r="B73" s="7"/>
-      <c r="C73" s="10"/>
-      <c r="D73" s="10"/>
-      <c r="E73" s="10"/>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="6"/>
-      <c r="B74" s="6"/>
-      <c r="C74" s="6"/>
-      <c r="D74" s="6"/>
-      <c r="E74" s="6"/>
-    </row>
-    <row r="75" spans="1:5" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="7"/>
-      <c r="B75" s="7"/>
-      <c r="C75" s="10"/>
-      <c r="D75" s="10"/>
-      <c r="E75" s="10"/>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="6"/>
-      <c r="B76" s="6"/>
-      <c r="C76" s="6"/>
-      <c r="D76" s="6"/>
-      <c r="E76" s="6"/>
-    </row>
-    <row r="77" spans="1:5" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="7"/>
-      <c r="B77" s="7"/>
-      <c r="C77" s="10"/>
-      <c r="D77" s="10"/>
-      <c r="E77" s="10"/>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="6"/>
-      <c r="B78" s="6"/>
-      <c r="C78" s="6"/>
-      <c r="D78" s="6"/>
-      <c r="E78" s="6"/>
-    </row>
-    <row r="79" spans="1:5" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="7"/>
-      <c r="B79" s="7"/>
-      <c r="C79" s="10"/>
-      <c r="D79" s="10"/>
-      <c r="E79" s="10"/>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="6"/>
-      <c r="B80" s="6"/>
-      <c r="C80" s="6"/>
-      <c r="D80" s="6"/>
-      <c r="E80" s="6"/>
-    </row>
-    <row r="81" spans="1:5" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="7"/>
-      <c r="B81" s="7"/>
-      <c r="C81" s="10"/>
-      <c r="D81" s="10"/>
-      <c r="E81" s="10"/>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="6"/>
-      <c r="B82" s="6"/>
-      <c r="C82" s="6"/>
-      <c r="D82" s="6"/>
-      <c r="E82" s="6"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>